<commit_message>
second commit removes public folder
</commit_message>
<xml_diff>
--- a/tasks.xlsx
+++ b/tasks.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Id</t>
   </si>
@@ -25,28 +25,31 @@
     <t>TaskType</t>
   </si>
   <si>
-    <t>"5f054e69cb3c572d84a8deb4"</t>
-  </si>
-  <si>
-    <t>qwer</t>
-  </si>
-  <si>
-    <t>Marketing</t>
+    <t>"5f0553090269c12d1c8ee6e7"</t>
+  </si>
+  <si>
+    <t>thej</t>
+  </si>
+  <si>
+    <t>Developer</t>
   </si>
   <si>
     <t>Pending</t>
   </si>
   <si>
-    <t>"5f05501fcb3c572d84a8deb5"</t>
-  </si>
-  <si>
-    <t>"5f0553090269c12d1c8ee6e7"</t>
-  </si>
-  <si>
-    <t>thej</t>
-  </si>
-  <si>
-    <t>Developer</t>
+    <t>"5f05accff6b3bb22dcc17178"</t>
+  </si>
+  <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>"5f05af8104dfeb226c3c42e0"</t>
+  </si>
+  <si>
+    <t>Efehi</t>
   </si>
 </sst>
 </file>
@@ -426,10 +429,7 @@
   <dimension ref="A1:D4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="40" customWidth="1"/>
-    <col min="4" max="4" width="60" outlineLevel="1" collapsed="1" customWidth="1"/>
+    <col min="1" max="4" width="100" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -468,21 +468,21 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>

</xml_diff>